<commit_message>
removed error of please activate your account
</commit_message>
<xml_diff>
--- a/GG Test cases.xlsx
+++ b/GG Test cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pgupta23\Desktop\Personal\GG auto clicker\GG-autoclicker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386F239C-85A5-4CED-A36D-C60C24920B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA5E6B6-E93B-4466-8573-2D50FD71ABB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{A041EC42-D3A6-4004-AB5C-981FD4F411F3}"/>
   </bookViews>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3485002-7E65-4150-9FDD-BDBF9A4FFAB0}">
   <dimension ref="B3:J94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F8" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>